<commit_message>
Fixed an issue with LPIII - it is the mean of the logs not the log of the mean, sd, skew...
Former-commit-id: 42f59fa3a2ff742963cc41a628ed892bf6d2bde9
</commit_message>
<xml_diff>
--- a/StatisticsTests/ExcelTesting/ExcelData/LogNormal.xlsx
+++ b/StatisticsTests/ExcelTesting/ExcelData/LogNormal.xlsx
@@ -17603,7 +17603,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="G8" s="11">
-        <x:v>43924.606944444444</x:v>
+        <x:v>44076.589583333334</x:v>
       </x:c>
       <x:c r="H8" s="7">
         <x:f>'Inverse CDF'!H9</x:f>
@@ -17658,7 +17658,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="G12" s="11">
-        <x:v>43924.60625</x:v>
+        <x:v>44076.589583333334</x:v>
       </x:c>
       <x:c r="H12" s="7">
         <x:f>'Inverse CDF'!H46</x:f>
@@ -17713,7 +17713,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="G16" s="11">
-        <x:v>43924.60625</x:v>
+        <x:v>44076.58888888889</x:v>
       </x:c>
       <x:c r="H16" s="7">
         <x:f>'Inverse CDF'!H83</x:f>
@@ -17768,7 +17768,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="G20" s="11">
-        <x:v>43924.606944444444</x:v>
+        <x:v>44076.589583333334</x:v>
       </x:c>
       <x:c r="H20" s="7">
         <x:f>'Inverse CDF'!H120</x:f>
@@ -17823,7 +17823,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="G24" s="11">
-        <x:v>43924.60625</x:v>
+        <x:v>44076.58888888889</x:v>
       </x:c>
       <x:c r="H24" s="7">
         <x:f>'Inverse CDF'!H157</x:f>

</xml_diff>

<commit_message>
Delete Old Tests Statistics Fix #67
</commit_message>
<xml_diff>
--- a/StatisticsTests/ExcelTesting/ExcelData/LogNormal.xlsx
+++ b/StatisticsTests/ExcelTesting/ExcelData/LogNormal.xlsx
@@ -17594,16 +17594,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D8" s="7" t="n">
-        <x:v>0.002484194007735488</x:v>
+        <x:v>0.00248419400773549</x:v>
       </x:c>
       <x:c r="E8" s="0" t="n">
-        <x:v>0.0024841940077354858</x:v>
+        <x:v>0.00248419400773549</x:v>
       </x:c>
       <x:c r="F8" s="35" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="G8" s="11">
-        <x:v>44078.811111111114</x:v>
+        <x:v>44431.56875</x:v>
       </x:c>
       <x:c r="H8" s="7">
         <x:f>'Inverse CDF'!H9</x:f>
@@ -17649,16 +17649,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D12" s="7" t="n">
-        <x:v>0.018355848883784883</x:v>
+        <x:v>0.0183558488837849</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>0.018355848883784866</x:v>
+        <x:v>0.0183558488837849</x:v>
       </x:c>
       <x:c r="F12" s="35" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="G12" s="11">
-        <x:v>44078.811111111114</x:v>
+        <x:v>44431.56875</x:v>
       </x:c>
       <x:c r="H12" s="7">
         <x:f>'Inverse CDF'!H46</x:f>
@@ -17704,16 +17704,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D16" s="7" t="n">
-        <x:v>1.9002511105560245E-12</x:v>
+        <x:v>1.90025111055602E-12</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>1.9002511105560177E-12</x:v>
+        <x:v>1.90025111055602E-12</x:v>
       </x:c>
       <x:c r="F16" s="35" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="G16" s="11">
-        <x:v>44078.811111111114</x:v>
+        <x:v>44431.56875</x:v>
       </x:c>
       <x:c r="H16" s="7">
         <x:f>'Inverse CDF'!H83</x:f>
@@ -17759,16 +17759,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D20" s="7" t="n">
-        <x:v>1.2653780950207851E-126</x:v>
+        <x:v>1.26537809502079E-126</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>1.2653780950207131E-126</x:v>
+        <x:v>1.26537809502071E-126</x:v>
       </x:c>
       <x:c r="F20" s="35" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="G20" s="11">
-        <x:v>44078.811111111114</x:v>
+        <x:v>44431.56875</x:v>
       </x:c>
       <x:c r="H20" s="7">
         <x:f>'Inverse CDF'!H120</x:f>
@@ -17814,16 +17814,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D24" s="7" t="n">
-        <x:v>7.3971625870362985</x:v>
+        <x:v>7.3971625870363</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>7.397162587036295</x:v>
+        <x:v>7.39716258703629</x:v>
       </x:c>
       <x:c r="F24" s="35" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="G24" s="11">
-        <x:v>44078.811111111114</x:v>
+        <x:v>44431.56875</x:v>
       </x:c>
       <x:c r="H24" s="7">
         <x:f>'Inverse CDF'!H157</x:f>
@@ -18451,7 +18451,7 @@
         <x:v>0.15</x:v>
       </x:c>
       <x:c r="D13" s="7" t="n">
-        <x:v>0.43983717963167834</x:v>
+        <x:v>0.439837179631678</x:v>
       </x:c>
       <x:c r="F13" s="7" t="str">
         <x:f>IF(ABS(E13 - D13) &lt;= (D13 * 0.01), "Passed", "Failed")</x:f>
@@ -18625,7 +18625,7 @@
         <x:v>0.25</x:v>
       </x:c>
       <x:c r="D17" s="7" t="n">
-        <x:v>0.6104553041901829</x:v>
+        <x:v>0.610455304190183</x:v>
       </x:c>
       <x:c r="F17" s="7" t="str">
         <x:f>IF(ABS(E17 - D17) &lt;= (D17 * 0.01), "Passed", "Failed")</x:f>
@@ -18678,7 +18678,7 @@
         <x:v>0.8</x:v>
       </x:c>
       <x:c r="D21" s="7" t="n">
-        <x:v>0.4864157811115534</x:v>
+        <x:v>0.486415781111553</x:v>
       </x:c>
       <x:c r="F21" s="7" t="str">
         <x:f>IF(ABS(E21 - D21) &lt;= (D21 * 0.01), "Passed", "Failed")</x:f>
@@ -18731,7 +18731,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D25" s="7" t="n">
-        <x:v>0.07272825613999476</x:v>
+        <x:v>0.0727282561399948</x:v>
       </x:c>
       <x:c r="F25" s="7" t="str">
         <x:f>IF(ABS(E25 - D25) &lt;= (D25 * 0.01), "Passed", "Failed")</x:f>
@@ -18788,7 +18788,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D30" s="7" t="n">
-        <x:v>0.02123058983158675</x:v>
+        <x:v>0.0212305898315867</x:v>
       </x:c>
       <x:c r="F30" s="7" t="str">
         <x:f>IF(ABS(E30 - D30) &lt;= (D30 * 0.01), "Passed", "Failed")</x:f>
@@ -18841,7 +18841,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D34" s="7" t="n">
-        <x:v>0.053990966513188056</x:v>
+        <x:v>0.0539909665131881</x:v>
       </x:c>
       <x:c r="F34" s="7" t="str">
         <x:f>IF(ABS(E34 - D34) &lt;= (D34 * 0.01), "Passed", "Failed")</x:f>
@@ -18894,7 +18894,7 @@
         <x:v>1.3</x:v>
       </x:c>
       <x:c r="D38" s="7" t="n">
-        <x:v>0.06781365030474373</x:v>
+        <x:v>0.0678136503047437</x:v>
       </x:c>
       <x:c r="F38" s="7" t="str">
         <x:f>IF(ABS(E38 - D38) &lt;= (D38 * 0.01), "Passed", "Failed")</x:f>
@@ -18950,7 +18950,7 @@
         <x:v>1.9</x:v>
       </x:c>
       <x:c r="D42" s="7" t="n">
-        <x:v>0.08348628996605717</x:v>
+        <x:v>0.0834862899660572</x:v>
       </x:c>
       <x:c r="E42" s="0" t="s"/>
       <x:c r="F42" s="7" t="str">
@@ -19020,7 +19020,7 @@
         <x:v>2.2</x:v>
       </x:c>
       <x:c r="D46" s="7" t="n">
-        <x:v>0.08704642539746184</x:v>
+        <x:v>0.0870464253974618</x:v>
       </x:c>
       <x:c r="F46" s="7" t="str">
         <x:f>IF(ABS(E46 - D46) &lt;= (D46 * 0.01), "Passed", "Failed")</x:f>
@@ -19077,7 +19077,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D51" s="7" t="n">
-        <x:v>0.03586637597255258</x:v>
+        <x:v>0.0358663759725526</x:v>
       </x:c>
       <x:c r="F51" s="7" t="str">
         <x:f>IF(ABS(E51 - D51) &lt;= (D51 * 0.01), "Passed", "Failed")</x:f>
@@ -19130,7 +19130,7 @@
         <x:v>2.75</x:v>
       </x:c>
       <x:c r="D55" s="7" t="n">
-        <x:v>0.026808079151839134</x:v>
+        <x:v>0.0268080791518391</x:v>
       </x:c>
       <x:c r="F55" s="7" t="str">
         <x:f>IF(ABS(E55 - D55) &lt;= (D55 * 0.01), "Passed", "Failed")</x:f>
@@ -19183,7 +19183,7 @@
         <x:v>3.2</x:v>
       </x:c>
       <x:c r="D59" s="7" t="n">
-        <x:v>0.02330685969113888</x:v>
+        <x:v>0.0233068596911389</x:v>
       </x:c>
       <x:c r="F59" s="7" t="str">
         <x:f>IF(ABS(E59 - D59) &lt;= (D59 * 0.01), "Passed", "Failed")</x:f>
@@ -19236,7 +19236,7 @@
         <x:v>3.4</x:v>
       </x:c>
       <x:c r="D63" s="7" t="n">
-        <x:v>0.02203217593478773</x:v>
+        <x:v>0.0220321759347877</x:v>
       </x:c>
       <x:c r="F63" s="7" t="str">
         <x:f>IF(ABS(E63 - D63) &lt;= (D63 * 0.01), "Passed", "Failed")</x:f>
@@ -19289,7 +19289,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D67" s="7" t="n">
-        <x:v>0.015352336271071444</x:v>
+        <x:v>0.0153523362710714</x:v>
       </x:c>
       <x:c r="F67" s="7" t="str">
         <x:f>IF(ABS(E67 - D67) &lt;= (D67 * 0.01), "Passed", "Failed")</x:f>
@@ -19346,7 +19346,7 @@
         <x:v>0.1</x:v>
       </x:c>
       <x:c r="D72" s="7" t="n">
-        <x:v>0.07740939172487982</x:v>
+        <x:v>0.0774093917248798</x:v>
       </x:c>
       <x:c r="F72" s="7" t="str">
         <x:f>IF(ABS(E72 - D72) &lt;= (D72 * 0.01), "Passed", "Failed")</x:f>
@@ -19399,7 +19399,7 @@
         <x:v>0.8</x:v>
       </x:c>
       <x:c r="D76" s="7" t="n">
-        <x:v>0.009767248108236096</x:v>
+        <x:v>0.0097672481082361</x:v>
       </x:c>
       <x:c r="F76" s="7" t="str">
         <x:f>IF(ABS(E76 - D76) &lt;= (D76 * 0.01), "Passed", "Failed")</x:f>
@@ -19452,7 +19452,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D80" s="7" t="n">
-        <x:v>0.002617800630021383</x:v>
+        <x:v>0.00261780063002138</x:v>
       </x:c>
       <x:c r="F80" s="7" t="str">
         <x:f>IF(ABS(E80 - D80) &lt;= (D80 * 0.01), "Passed", "Failed")</x:f>
@@ -19505,7 +19505,7 @@
         <x:v>5.5</x:v>
       </x:c>
       <x:c r="D84" s="7" t="n">
-        <x:v>0.0014308710822864199</x:v>
+        <x:v>0.00143087108228642</x:v>
       </x:c>
       <x:c r="F84" s="7" t="str">
         <x:f>IF(ABS(E84 - D84) &lt;= (D84 * 0.01), "Passed", "Failed")</x:f>
@@ -19558,7 +19558,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="D88" s="7" t="n">
-        <x:v>0.0006574357521596822</x:v>
+        <x:v>0.000657435752159682</x:v>
       </x:c>
       <x:c r="F88" s="7" t="str">
         <x:f>IF(ABS(E88 - D88) &lt;= (D88 * 0.01), "Passed", "Failed")</x:f>
@@ -19615,7 +19615,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D93" s="7" t="n">
-        <x:v>1.6002110268672838E-14</x:v>
+        <x:v>1.60021102686728E-14</x:v>
       </x:c>
       <x:c r="F93" s="7" t="str">
         <x:f>IF(ABS(E93 - D93) &lt;= (D93 * 0.01), "Passed", "Failed")</x:f>
@@ -19668,7 +19668,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="D97" s="7" t="n">
-        <x:v>1.4558664808870748E-06</x:v>
+        <x:v>1.45586648088707E-06</x:v>
       </x:c>
       <x:c r="F97" s="7" t="str">
         <x:f>IF(ABS(E97 - D97) &lt;= (D97 * 0.01), "Passed", "Failed")</x:f>
@@ -19721,7 +19721,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="D101" s="7" t="n">
-        <x:v>0.00016016142275285838</x:v>
+        <x:v>0.000160161422752858</x:v>
       </x:c>
       <x:c r="F101" s="7" t="str">
         <x:f>IF(ABS(E101 - D101) &lt;= (D101 * 0.01), "Passed", "Failed")</x:f>
@@ -19774,7 +19774,7 @@
         <x:v>55</x:v>
       </x:c>
       <x:c r="D105" s="7" t="n">
-        <x:v>0.0020215325883079097</x:v>
+        <x:v>0.00202153258830791</x:v>
       </x:c>
       <x:c r="F105" s="7" t="str">
         <x:f>IF(ABS(E105 - D105) &lt;= (D105 * 0.01), "Passed", "Failed")</x:f>
@@ -19827,7 +19827,7 @@
         <x:v>250</x:v>
       </x:c>
       <x:c r="D109" s="7" t="n">
-        <x:v>0.0018527296363705795</x:v>
+        <x:v>0.00185272963637058</x:v>
       </x:c>
       <x:c r="F109" s="7" t="str">
         <x:f>IF(ABS(E109 - D109) &lt;= (D109 * 0.01), "Passed", "Failed")</x:f>
@@ -19979,7 +19979,7 @@
         <x:v>0.01</x:v>
       </x:c>
       <x:c r="D9" s="7" t="n">
-        <x:v>2.0606433959717215E-06</x:v>
+        <x:v>2.06064339597172E-06</x:v>
       </x:c>
       <x:c r="F9" s="7" t="str">
         <x:f>IF(ABS(E9 - D9) &lt;= (D9 * 0.01), "Passed", "Failed")</x:f>
@@ -20106,7 +20106,7 @@
         <x:v>0.15</x:v>
       </x:c>
       <x:c r="D13" s="7" t="n">
-        <x:v>0.028906052073384945</x:v>
+        <x:v>0.0289060520733849</x:v>
       </x:c>
       <x:c r="F13" s="7" t="str">
         <x:f>IF(ABS(E13 - D13) &lt;= (D13 * 0.01), "Passed", "Failed")</x:f>
@@ -20280,7 +20280,7 @@
         <x:v>0.25</x:v>
       </x:c>
       <x:c r="D17" s="7" t="n">
-        <x:v>0.08282851900169848</x:v>
+        <x:v>0.0828285190016985</x:v>
       </x:c>
       <x:c r="F17" s="7" t="str">
         <x:f>IF(ABS(E17 - D17) &lt;= (D17 * 0.01), "Passed", "Failed")</x:f>
@@ -20333,7 +20333,7 @@
         <x:v>0.8</x:v>
       </x:c>
       <x:c r="D21" s="7" t="n">
-        <x:v>0.41171189185745494</x:v>
+        <x:v>0.411711891857455</x:v>
       </x:c>
       <x:c r="F21" s="7" t="str">
         <x:f>IF(ABS(E21 - D21) &lt;= (D21 * 0.01), "Passed", "Failed")</x:f>
@@ -20386,7 +20386,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D25" s="7" t="n">
-        <x:v>0.8640313923585755</x:v>
+        <x:v>0.864031392358576</x:v>
       </x:c>
       <x:c r="F25" s="7" t="str">
         <x:f>IF(ABS(E25 - D25) &lt;= (D25 * 0.01), "Passed", "Failed")</x:f>
@@ -20443,7 +20443,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D30" s="7" t="n">
-        <x:v>0.003539050776086408</x:v>
+        <x:v>0.00353905077608641</x:v>
       </x:c>
       <x:c r="F30" s="7" t="str">
         <x:f>IF(ABS(E30 - D30) &lt;= (D30 * 0.01), "Passed", "Failed")</x:f>
@@ -20496,7 +20496,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D34" s="7" t="n">
-        <x:v>0.02275013194817919</x:v>
+        <x:v>0.0227501319481792</x:v>
       </x:c>
       <x:c r="F34" s="7" t="str">
         <x:f>IF(ABS(E34 - D34) &lt;= (D34 * 0.01), "Passed", "Failed")</x:f>
@@ -20549,7 +20549,7 @@
         <x:v>1.3</x:v>
       </x:c>
       <x:c r="D38" s="7" t="n">
-        <x:v>0.041137509460306004</x:v>
+        <x:v>0.041137509460306</x:v>
       </x:c>
       <x:c r="F38" s="7" t="str">
         <x:f>IF(ABS(E38 - D38) &lt;= (D38 * 0.01), "Passed", "Failed")</x:f>
@@ -20671,7 +20671,7 @@
         <x:v>2.2</x:v>
       </x:c>
       <x:c r="D46" s="7" t="n">
-        <x:v>0.11284375153914879</x:v>
+        <x:v>0.112843751539149</x:v>
       </x:c>
       <x:c r="F46" s="7" t="str">
         <x:f>IF(ABS(E46 - D46) &lt;= (D46 * 0.01), "Passed", "Failed")</x:f>
@@ -20728,7 +20728,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D51" s="7" t="n">
-        <x:v>0.3222663833548772</x:v>
+        <x:v>0.322266383354877</x:v>
       </x:c>
       <x:c r="F51" s="7" t="str">
         <x:f>IF(ABS(E51 - D51) &lt;= (D51 * 0.01), "Passed", "Failed")</x:f>
@@ -20781,7 +20781,7 @@
         <x:v>2.75</x:v>
       </x:c>
       <x:c r="D55" s="7" t="n">
-        <x:v>0.34543310811726136</x:v>
+        <x:v>0.345433108117261</x:v>
       </x:c>
       <x:c r="F55" s="7" t="str">
         <x:f>IF(ABS(E55 - D55) &lt;= (D55 * 0.01), "Passed", "Failed")</x:f>
@@ -20887,7 +20887,7 @@
         <x:v>3.4</x:v>
       </x:c>
       <x:c r="D63" s="7" t="n">
-        <x:v>0.3612030599463717</x:v>
+        <x:v>0.361203059946372</x:v>
       </x:c>
       <x:c r="F63" s="7" t="str">
         <x:f>IF(ABS(E63 - D63) &lt;= (D63 * 0.01), "Passed", "Failed")</x:f>
@@ -20940,7 +20940,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D67" s="7" t="n">
-        <x:v>0.39046303191541964</x:v>
+        <x:v>0.39046303191542</x:v>
       </x:c>
       <x:c r="F67" s="7" t="str">
         <x:f>IF(ABS(E67 - D67) &lt;= (D67 * 0.01), "Passed", "Failed")</x:f>
@@ -20997,7 +20997,7 @@
         <x:v>0.1</x:v>
       </x:c>
       <x:c r="D72" s="7" t="n">
-        <x:v>0.40282110507592256</x:v>
+        <x:v>0.402821105075923</x:v>
       </x:c>
       <x:c r="F72" s="7" t="str">
         <x:f>IF(ABS(E72 - D72) &lt;= (D72 * 0.01), "Passed", "Failed")</x:f>
@@ -21050,7 +21050,7 @@
         <x:v>0.8</x:v>
       </x:c>
       <x:c r="D76" s="7" t="n">
-        <x:v>0.4189959018577607</x:v>
+        <x:v>0.418995901857761</x:v>
       </x:c>
       <x:c r="F76" s="7" t="str">
         <x:f>IF(ABS(E76 - D76) &lt;= (D76 * 0.01), "Passed", "Failed")</x:f>
@@ -21103,7 +21103,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D80" s="7" t="n">
-        <x:v>0.42935058958839695</x:v>
+        <x:v>0.429350589588397</x:v>
       </x:c>
       <x:c r="F80" s="7" t="str">
         <x:f>IF(ABS(E80 - D80) &lt;= (D80 * 0.01), "Passed", "Failed")</x:f>
@@ -21209,7 +21209,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="D88" s="7" t="n">
-        <x:v>0.4402632300336503</x:v>
+        <x:v>0.44026323003365</x:v>
       </x:c>
       <x:c r="F88" s="7" t="str">
         <x:f>IF(ABS(E88 - D88) &lt;= (D88 * 0.01), "Passed", "Failed")</x:f>
@@ -21266,7 +21266,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D93" s="7" t="n">
-        <x:v>3.028013344369828E-15</x:v>
+        <x:v>3.02801334436983E-15</x:v>
       </x:c>
       <x:c r="F93" s="7" t="str">
         <x:f>IF(ABS(E93 - D93) &lt;= (D93 * 0.01), "Passed", "Failed")</x:f>
@@ -21319,7 +21319,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="D97" s="7" t="n">
-        <x:v>2.2819172148093587E-06</x:v>
+        <x:v>2.28191721480936E-06</x:v>
       </x:c>
       <x:c r="F97" s="7" t="str">
         <x:f>IF(ABS(E97 - D97) &lt;= (D97 * 0.01), "Passed", "Failed")</x:f>
@@ -21372,7 +21372,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="D101" s="7" t="n">
-        <x:v>0.0006928691913806522</x:v>
+        <x:v>0.000692869191380652</x:v>
       </x:c>
       <x:c r="F101" s="7" t="str">
         <x:f>IF(ABS(E101 - D101) &lt;= (D101 * 0.01), "Passed", "Failed")</x:f>
@@ -21425,7 +21425,7 @@
         <x:v>55</x:v>
       </x:c>
       <x:c r="D105" s="7" t="n">
-        <x:v>0.023553682423743876</x:v>
+        <x:v>0.0235536824237439</x:v>
       </x:c>
       <x:c r="F105" s="7" t="str">
         <x:f>IF(ABS(E105 - D105) &lt;= (D105 * 0.01), "Passed", "Failed")</x:f>
@@ -21478,7 +21478,7 @@
         <x:v>250</x:v>
       </x:c>
       <x:c r="D109" s="7" t="n">
-        <x:v>0.8515077521992471</x:v>
+        <x:v>0.851507752199247</x:v>
       </x:c>
       <x:c r="F109" s="7" t="str">
         <x:f>IF(ABS(E109 - D109) &lt;= (D109 * 0.01), "Passed", "Failed")</x:f>
@@ -21621,7 +21621,7 @@
         <x:v>1E-09</x:v>
       </x:c>
       <x:c r="D9" s="7" t="n">
-        <x:v>0.002484194007735488</x:v>
+        <x:v>0.00248419400773549</x:v>
       </x:c>
       <x:c r="F9" s="7" t="str">
         <x:f>IF(ABS(E9 - D9) &lt;= (ABS(H9) * 0.01), "Passed", "Failed")</x:f>
@@ -21739,7 +21739,7 @@
         <x:v>0.01</x:v>
       </x:c>
       <x:c r="D13" s="7" t="n">
-        <x:v>0.09765173307033599</x:v>
+        <x:v>0.097651733070336</x:v>
       </x:c>
       <x:c r="F13" s="7" t="str">
         <x:f>IF(ABS(E13 - D13) &lt;= (ABS(H13) * 0.01), "Passed", "Failed")</x:f>
@@ -21866,7 +21866,7 @@
         <x:v>0.05</x:v>
       </x:c>
       <x:c r="D17" s="7" t="n">
-        <x:v>0.19304081669873657</x:v>
+        <x:v>0.193040816698737</x:v>
       </x:c>
       <x:c r="F17" s="7" t="str">
         <x:f>IF(ABS(E17 - D17) &lt;= (ABS(H17) * 0.01), "Passed", "Failed")</x:f>
@@ -21974,7 +21974,7 @@
         <x:v>0.25</x:v>
       </x:c>
       <x:c r="D21" s="7" t="n">
-        <x:v>0.5094162838632774</x:v>
+        <x:v>0.509416283863277</x:v>
       </x:c>
       <x:c r="F21" s="7" t="str">
         <x:f>IF(ABS(E21 - D21) &lt;= (ABS(H21) * 0.01), "Passed", "Failed")</x:f>
@@ -22080,7 +22080,7 @@
         <x:v>0.75</x:v>
       </x:c>
       <x:c r="D29" s="7" t="n">
-        <x:v>1.9630310841582574</x:v>
+        <x:v>1.96303108415826</x:v>
       </x:c>
       <x:c r="F29" s="7" t="str">
         <x:f>IF(ABS(E29 - D29) &lt;= (ABS(H29) * 0.01), "Passed", "Failed")</x:f>
@@ -22186,7 +22186,7 @@
         <x:v>0.99</x:v>
       </x:c>
       <x:c r="D37" s="7" t="n">
-        <x:v>10.240473656312131</x:v>
+        <x:v>10.2404736563121</x:v>
       </x:c>
       <x:c r="F37" s="7" t="str">
         <x:f>IF(ABS(E37 - D37) &lt;= (ABS(H37) * 0.01), "Passed", "Failed")</x:f>
@@ -22239,7 +22239,7 @@
         <x:v>0.999999999</x:v>
       </x:c>
       <x:c r="D41" s="7" t="n">
-        <x:v>402.5450514251582</x:v>
+        <x:v>402.545051425158</x:v>
       </x:c>
       <x:c r="F41" s="7" t="str">
         <x:f>IF(ABS(E41 - D41) &lt;= (ABS(H41) * 0.01), "Passed", "Failed")</x:f>
@@ -22306,7 +22306,7 @@
         <x:v>1E-09</x:v>
       </x:c>
       <x:c r="D46" s="7" t="n">
-        <x:v>0.018355848883784883</x:v>
+        <x:v>0.0183558488837849</x:v>
       </x:c>
       <x:c r="F46" s="7" t="str">
         <x:f>IF(ABS(E46 - D46) &lt;= (ABS(H46) * 0.01), "Passed", "Failed")</x:f>
@@ -22414,7 +22414,7 @@
         <x:v>0.05</x:v>
       </x:c>
       <x:c r="D54" s="7" t="n">
-        <x:v>1.4263894239703532</x:v>
+        <x:v>1.42638942397035</x:v>
       </x:c>
       <x:c r="F54" s="7" t="str">
         <x:f>IF(ABS(E54 - D54) &lt;= (ABS(H54) * 0.01), "Passed", "Failed")</x:f>
@@ -22466,7 +22466,7 @@
         <x:v>0.25</x:v>
       </x:c>
       <x:c r="D58" s="7" t="n">
-        <x:v>3.7641054991745366</x:v>
+        <x:v>3.76410549917454</x:v>
       </x:c>
       <x:c r="F58" s="7" t="str">
         <x:f>IF(ABS(E58 - D58) &lt;= (ABS(H58) * 0.01), "Passed", "Failed")</x:f>
@@ -22570,7 +22570,7 @@
         <x:v>0.75</x:v>
       </x:c>
       <x:c r="D66" s="7" t="n">
-        <x:v>14.50494680479002</x:v>
+        <x:v>14.50494680479</x:v>
       </x:c>
       <x:c r="F66" s="7" t="str">
         <x:f>IF(ABS(E66 - D66) &lt;= (ABS(H66) * 0.01), "Passed", "Failed")</x:f>
@@ -22622,7 +22622,7 @@
         <x:v>0.95</x:v>
       </x:c>
       <x:c r="D70" s="7" t="n">
-        <x:v>38.277169695475095</x:v>
+        <x:v>38.2771696954751</x:v>
       </x:c>
       <x:c r="F70" s="7" t="str">
         <x:f>IF(ABS(E70 - D70) &lt;= (ABS(H70) * 0.01), "Passed", "Failed")</x:f>
@@ -22674,7 +22674,7 @@
         <x:v>0.99</x:v>
       </x:c>
       <x:c r="D74" s="7" t="n">
-        <x:v>75.66743432611182</x:v>
+        <x:v>75.6674343261118</x:v>
       </x:c>
       <x:c r="F74" s="7" t="str">
         <x:f>IF(ABS(E74 - D74) &lt;= (ABS(H74) * 0.01), "Passed", "Failed")</x:f>
@@ -22726,7 +22726,7 @@
         <x:v>0.999999999</x:v>
       </x:c>
       <x:c r="D78" s="7" t="n">
-        <x:v>2974.4279673274173</x:v>
+        <x:v>2974.42796732742</x:v>
       </x:c>
       <x:c r="F78" s="7" t="str">
         <x:f>IF(ABS(E78 - D78) &lt;= (ABS(H78) * 0.01), "Passed", "Failed")</x:f>
@@ -22782,7 +22782,7 @@
         <x:v>1E-09</x:v>
       </x:c>
       <x:c r="D83" s="7" t="n">
-        <x:v>1.9002511105560245E-12</x:v>
+        <x:v>1.90025111055602E-12</x:v>
       </x:c>
       <x:c r="F83" s="7" t="str">
         <x:f>IF(ABS(E83 - D83) &lt;= (ABS(H83) * 0.01), "Passed", "Failed")</x:f>
@@ -22837,7 +22837,7 @@
         <x:v>0.01</x:v>
       </x:c>
       <x:c r="D87" s="7" t="n">
-        <x:v>0.0001783541513149171</x:v>
+        <x:v>0.000178354151314917</x:v>
       </x:c>
       <x:c r="F87" s="7" t="str">
         <x:f>IF(ABS(E87 - D87) &lt;= (ABS(H87) * 0.01), "Passed", "Failed")</x:f>
@@ -22890,7 +22890,7 @@
         <x:v>0.05</x:v>
       </x:c>
       <x:c r="D91" s="7" t="n">
-        <x:v>0.005384299099642256</x:v>
+        <x:v>0.00538429909964226</x:v>
       </x:c>
       <x:c r="F91" s="7" t="str">
         <x:f>IF(ABS(E91 - D91) &lt;= (ABS(H91) * 0.01), "Passed", "Failed")</x:f>
@@ -22942,7 +22942,7 @@
         <x:v>0.25</x:v>
       </x:c>
       <x:c r="D95" s="7" t="n">
-        <x:v>0.6890449635318557</x:v>
+        <x:v>0.689044963531856</x:v>
       </x:c>
       <x:c r="F95" s="7" t="str">
         <x:f>IF(ABS(E95 - D95) &lt;= (ABS(H95) * 0.01), "Passed", "Failed")</x:f>
@@ -22994,7 +22994,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D99" s="7" t="n">
-        <x:v>20.085536923187668</x:v>
+        <x:v>20.0855369231877</x:v>
       </x:c>
       <x:c r="F99" s="7" t="str">
         <x:f>IF(ABS(E99 - D99) &lt;= (ABS(H99) * 0.01), "Passed", "Failed")</x:f>
@@ -23046,7 +23046,7 @@
         <x:v>0.75</x:v>
       </x:c>
       <x:c r="D103" s="7" t="n">
-        <x:v>585.4897936193737</x:v>
+        <x:v>585.489793619374</x:v>
       </x:c>
       <x:c r="F103" s="7" t="str">
         <x:f>IF(ABS(E103 - D103) &lt;= (ABS(H103) * 0.01), "Passed", "Failed")</x:f>
@@ -23098,7 +23098,7 @@
         <x:v>0.95</x:v>
       </x:c>
       <x:c r="D107" s="7" t="n">
-        <x:v>74926.89132361492</x:v>
+        <x:v>74926.8913236149</x:v>
       </x:c>
       <x:c r="F107" s="7" t="str">
         <x:f>IF(ABS(E107 - D107) &lt;= (ABS(H107) * 0.01), "Passed", "Failed")</x:f>
@@ -23150,7 +23150,7 @@
         <x:v>0.99</x:v>
       </x:c>
       <x:c r="D111" s="7" t="n">
-        <x:v>2261953.4814213957</x:v>
+        <x:v>2261953.4814214</x:v>
       </x:c>
       <x:c r="F111" s="7" t="str">
         <x:f>IF(ABS(E111 - D111) &lt;= (ABS(H111) * 0.01), "Passed", "Failed")</x:f>
@@ -23202,7 +23202,7 @@
         <x:v>0.999999999</x:v>
       </x:c>
       <x:c r="D115" s="7" t="n">
-        <x:v>212302890138214.3</x:v>
+        <x:v>212302890138214</x:v>
       </x:c>
       <x:c r="F115" s="7" t="str">
         <x:f>IF(ABS(E115 - D115) &lt;= (ABS(H115) * 0.01), "Passed", "Failed")</x:f>
@@ -23258,7 +23258,7 @@
         <x:v>1E-09</x:v>
       </x:c>
       <x:c r="D120" s="7" t="n">
-        <x:v>1.2653780950207851E-126</x:v>
+        <x:v>1.26537809502079E-126</x:v>
       </x:c>
       <x:c r="F120" s="7" t="str">
         <x:f>IF(ABS(E120 - D120) &lt;= (ABS(H120) * 0.01), "Passed", "Failed")</x:f>
@@ -23313,7 +23313,7 @@
         <x:v>0.01</x:v>
       </x:c>
       <x:c r="D124" s="7" t="n">
-        <x:v>6.713400937314998E-47</x:v>
+        <x:v>6.713400937315E-47</x:v>
       </x:c>
       <x:c r="F124" s="7" t="str">
         <x:f>IF(ABS(E124 - D124) &lt;= (ABS(H124) * 0.01), "Passed", "Failed")</x:f>
@@ -23366,7 +23366,7 @@
         <x:v>0.05</x:v>
       </x:c>
       <x:c r="D128" s="7" t="n">
-        <x:v>4.220871520774463E-32</x:v>
+        <x:v>4.22087152077446E-32</x:v>
       </x:c>
       <x:c r="F128" s="7" t="str">
         <x:f>IF(ABS(E128 - D128) &lt;= (ABS(H128) * 0.01), "Passed", "Failed")</x:f>
@@ -23418,7 +23418,7 @@
         <x:v>0.25</x:v>
       </x:c>
       <x:c r="D132" s="7" t="n">
-        <x:v>4.9726281995865685E-11</x:v>
+        <x:v>4.97262819958657E-11</x:v>
       </x:c>
       <x:c r="F132" s="7" t="str">
         <x:f>IF(ABS(E132 - D132) &lt;= (ABS(H132) * 0.01), "Passed", "Failed")</x:f>
@@ -23470,7 +23470,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D136" s="7" t="n">
-        <x:v>22026.465794806718</x:v>
+        <x:v>22026.4657948067</x:v>
       </x:c>
       <x:c r="F136" s="7" t="str">
         <x:f>IF(ABS(E136 - D136) &lt;= (ABS(H136) * 0.01), "Passed", "Failed")</x:f>
@@ -23522,7 +23522,7 @@
         <x:v>0.75</x:v>
       </x:c>
       <x:c r="D140" s="7" t="n">
-        <x:v>9.756715683069321E+18</x:v>
+        <x:v>9.75671568306932E+18</x:v>
       </x:c>
       <x:c r="F140" s="7" t="str">
         <x:f>IF(ABS(E140 - D140) &lt;= (ABS(H140) * 0.01), "Passed", "Failed")</x:f>
@@ -23574,7 +23574,7 @@
         <x:v>0.95</x:v>
       </x:c>
       <x:c r="D144" s="7" t="n">
-        <x:v>1.1494431731026548E+40</x:v>
+        <x:v>1.14944317310265E+40</x:v>
       </x:c>
       <x:c r="F144" s="7" t="str">
         <x:f>IF(ABS(E144 - D144) &lt;= (ABS(H144) * 0.01), "Passed", "Failed")</x:f>
@@ -23678,7 +23678,7 @@
         <x:v>0.999999999</x:v>
       </x:c>
       <x:c r="D152" s="7" t="n">
-        <x:v>3.834152880946759E+134</x:v>
+        <x:v>3.83415288094676E+134</x:v>
       </x:c>
       <x:c r="F152" s="7" t="str">
         <x:f>IF(ABS(E152 - D152) &lt;= (ABS(H152) * 0.01), "Passed", "Failed")</x:f>
@@ -23734,7 +23734,7 @@
         <x:v>1E-09</x:v>
       </x:c>
       <x:c r="D157" s="7" t="n">
-        <x:v>7.3971625870362985</x:v>
+        <x:v>7.3971625870363</x:v>
       </x:c>
       <x:c r="F157" s="7" t="str">
         <x:f>IF(ABS(E157 - D157) &lt;= (ABS(H157) * 0.01), "Passed", "Failed")</x:f>
@@ -23789,7 +23789,7 @@
         <x:v>0.01</x:v>
       </x:c>
       <x:c r="D161" s="7" t="n">
-        <x:v>46.37803961227072</x:v>
+        <x:v>46.3780396122707</x:v>
       </x:c>
       <x:c r="F161" s="7" t="str">
         <x:f>IF(ABS(E161 - D161) &lt;= (ABS(H161) * 0.01), "Passed", "Failed")</x:f>
@@ -23842,7 +23842,7 @@
         <x:v>0.05</x:v>
       </x:c>
       <x:c r="D165" s="7" t="n">
-        <x:v>65.20741480856508</x:v>
+        <x:v>65.2074148085651</x:v>
       </x:c>
       <x:c r="F165" s="7" t="str">
         <x:f>IF(ABS(E165 - D165) &lt;= (ABS(H165) * 0.01), "Passed", "Failed")</x:f>
@@ -23894,7 +23894,7 @@
         <x:v>0.25</x:v>
       </x:c>
       <x:c r="D169" s="7" t="n">
-        <x:v>105.92752405221233</x:v>
+        <x:v>105.927524052212</x:v>
       </x:c>
       <x:c r="F169" s="7" t="str">
         <x:f>IF(ABS(E169 - D169) &lt;= (ABS(H169) * 0.01), "Passed", "Failed")</x:f>
@@ -23946,7 +23946,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D173" s="7" t="n">
-        <x:v>148.4131591025766</x:v>
+        <x:v>148.413159102577</x:v>
       </x:c>
       <x:c r="F173" s="7" t="str">
         <x:f>IF(ABS(E173 - D173) &lt;= (ABS(H173) * 0.01), "Passed", "Failed")</x:f>
@@ -23998,7 +23998,7 @@
         <x:v>0.75</x:v>
       </x:c>
       <x:c r="D177" s="7" t="n">
-        <x:v>207.93902238241438</x:v>
+        <x:v>207.939022382414</x:v>
       </x:c>
       <x:c r="F177" s="7" t="str">
         <x:f>IF(ABS(E177 - D177) &lt;= (ABS(H177) * 0.01), "Passed", "Failed")</x:f>
@@ -24154,7 +24154,7 @@
         <x:v>0.999999999</x:v>
       </x:c>
       <x:c r="D189" s="7" t="n">
-        <x:v>2977.6911871590964</x:v>
+        <x:v>2977.6911871591</x:v>
       </x:c>
       <x:c r="F189" s="7" t="str">
         <x:f>IF(ABS(E189 - D189) &lt;= (ABS(H189) * 0.01), "Passed", "Failed")</x:f>
@@ -24892,7 +24892,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="E8" s="7" t="n">
-        <x:v>402.5450514251582</x:v>
+        <x:v>402.545051425158</x:v>
       </x:c>
       <x:c r="G8" s="7" t="str">
         <x:f>IF(ABS(F8 - E8) &lt;= (E8 * 0.01), "Passed", "Failed")</x:f>
@@ -24938,7 +24938,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="E12" s="7" t="n">
-        <x:v>2974.4279673274173</x:v>
+        <x:v>2974.42796732742</x:v>
       </x:c>
       <x:c r="G12" s="7" t="str">
         <x:f>IF(ABS(F12 - E12) &lt;= (E12 * 0.01), "Passed", "Failed")</x:f>
@@ -24984,7 +24984,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E16" s="7" t="n">
-        <x:v>212302890138214.3</x:v>
+        <x:v>212302890138214</x:v>
       </x:c>
       <x:c r="G16" s="7" t="str">
         <x:f>IF(ABS(F16 - E16) &lt;= (E16 * 0.01), "Passed", "Failed")</x:f>
@@ -25030,7 +25030,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="E20" s="7" t="n">
-        <x:v>3.834152880946759E+134</x:v>
+        <x:v>3.83415288094676E+134</x:v>
       </x:c>
       <x:c r="G20" s="7" t="str">
         <x:f>IF(ABS(F20 - E20) &lt;= (E20 * 0.01), "Passed", "Failed")</x:f>
@@ -25076,7 +25076,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="E24" s="7" t="n">
-        <x:v>2977.6911871590964</x:v>
+        <x:v>2977.6911871591</x:v>
       </x:c>
       <x:c r="G24" s="7" t="str">
         <x:f>IF(ABS(F24 - E24) &lt;= (E24 * 0.01), "Passed", "Failed")</x:f>
@@ -25215,7 +25215,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D8" s="7" t="n">
-        <x:v>0.36787944117144233</x:v>
+        <x:v>0.367879441171442</x:v>
       </x:c>
       <x:c r="F8" s="7" t="str">
         <x:f>IF(ABS(E8 - D8) &lt;= (D8 * 0.01), "Passed", "Failed")</x:f>
@@ -25261,7 +25261,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D12" s="7" t="n">
-        <x:v>2.718281828459045</x:v>
+        <x:v>2.71828182845905</x:v>
       </x:c>
       <x:c r="F12" s="7" t="str">
         <x:f>IF(ABS(E12 - D12) &lt;= (D12 * 0.01), "Passed", "Failed")</x:f>
@@ -25307,7 +25307,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D16" s="7" t="n">
-        <x:v>2.7894680928689246E-10</x:v>
+        <x:v>2.78946809286892E-10</x:v>
       </x:c>
       <x:c r="F16" s="7" t="str">
         <x:f>IF(ABS(E16 - D16) &lt;= (D16 * 0.01), "Passed", "Failed")</x:f>
@@ -25399,7 +25399,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D24" s="7" t="n">
-        <x:v>115.58428452718766</x:v>
+        <x:v>115.584284527188</x:v>
       </x:c>
       <x:c r="F24" s="7" t="str">
         <x:f>IF(ABS(E24 - D24) &lt;= (D24 * 0.01), "Passed", "Failed")</x:f>
@@ -25537,7 +25537,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D8" s="7" t="n">
-        <x:v>1.6487212707001282</x:v>
+        <x:v>1.64872127070013</x:v>
       </x:c>
       <x:c r="F8" s="7" t="str">
         <x:f>IF(ABS(E8 - D8) &lt;= (D8 * 0.01), "Passed", "Failed")</x:f>
@@ -25583,7 +25583,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D12" s="7" t="n">
-        <x:v>12.182493960703473</x:v>
+        <x:v>12.1824939607035</x:v>
       </x:c>
       <x:c r="F12" s="7" t="str">
         <x:f>IF(ABS(E12 - D12) &lt;= (D12 * 0.01), "Passed", "Failed")</x:f>
@@ -25629,7 +25629,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D16" s="7" t="n">
-        <x:v>5389698.476283012</x:v>
+        <x:v>5389698.47628301</x:v>
       </x:c>
       <x:c r="F16" s="7" t="str">
         <x:f>IF(ABS(E16 - D16) &lt;= (D16 * 0.01), "Passed", "Failed")</x:f>
@@ -25718,7 +25718,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D24" s="7" t="n">
-        <x:v>168.17414165184545</x:v>
+        <x:v>168.174141651845</x:v>
       </x:c>
       <x:c r="F24" s="7" t="str">
         <x:f>IF(ABS(E24 - D24) &lt;= (D24 * 0.01), "Passed", "Failed")</x:f>
@@ -25948,7 +25948,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D16" s="7" t="n">
-        <x:v>20.085536923187668</x:v>
+        <x:v>20.0855369231877</x:v>
       </x:c>
       <x:c r="F16" s="7" t="str">
         <x:f>IF(ABS(E16 - D16) &lt;= (D16 * 0.01), "Passed", "Failed")</x:f>
@@ -25994,7 +25994,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="D20" s="7" t="n">
-        <x:v>22026.465794806718</x:v>
+        <x:v>22026.4657948067</x:v>
       </x:c>
       <x:c r="F20" s="7" t="str">
         <x:f>IF(ABS(E20 - D20) &lt;= (D20 * 0.01), "Passed", "Failed")</x:f>
@@ -26040,7 +26040,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D24" s="7" t="n">
-        <x:v>148.4131591025766</x:v>
+        <x:v>148.413159102577</x:v>
       </x:c>
       <x:c r="F24" s="7" t="str">
         <x:f>IF(ABS(E24 - D24) &lt;= (D24 * 0.01), "Passed", "Failed")</x:f>
@@ -26178,7 +26178,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D8" s="7" t="n">
-        <x:v>4.670774270471604</x:v>
+        <x:v>4.6707742704716</x:v>
       </x:c>
       <x:c r="F8" s="7" t="str">
         <x:f>IF(ABS(E8 - D8) &lt;= (D8 * 0.01), "Passed", "Failed")</x:f>
@@ -26224,7 +26224,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D12" s="7" t="n">
-        <x:v>255.01563439015848</x:v>
+        <x:v>255.015634390158</x:v>
       </x:c>
       <x:c r="F12" s="7" t="str">
         <x:f>IF(ABS(E12 - D12) &lt;= (D12 * 0.01), "Passed", "Failed")</x:f>
@@ -26270,7 +26270,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D16" s="7" t="n">
-        <x:v>2.0916594959839476E+24</x:v>
+        <x:v>2.09165949598395E+24</x:v>
       </x:c>
       <x:c r="F16" s="7" t="str">
         <x:f>IF(ABS(E16 - D16) &lt;= (D16 * 0.01), "Passed", "Failed")</x:f>
@@ -26359,7 +26359,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D24" s="7" t="n">
-        <x:v>8032.960753911656</x:v>
+        <x:v>8032.96075391166</x:v>
       </x:c>
       <x:c r="F24" s="7" t="str">
         <x:f>IF(ABS(E24 - D24) &lt;= (D24 * 0.01), "Passed", "Failed")</x:f>
@@ -35010,7 +35010,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D8" s="7" t="n">
-        <x:v>4.874044644200469</x:v>
+        <x:v>4.87404464420047</x:v>
       </x:c>
       <x:c r="F8" s="7" t="str">
         <x:f>IF(ABS(E8 - D8) &lt;= (D8 * 0.01), "Passed", "Failed")</x:f>
@@ -35056,7 +35056,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D12" s="7" t="n">
-        <x:v>4.874044644200469</x:v>
+        <x:v>4.87404464420047</x:v>
       </x:c>
       <x:c r="F12" s="7" t="str">
         <x:f>IF(ABS(E12 - D12) &lt;= (D12 * 0.01), "Passed", "Failed")</x:f>
@@ -35102,7 +35102,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D16" s="7" t="n">
-        <x:v>19321599304537008</x:v>
+        <x:v>1.9321599304537E+16</x:v>
       </x:c>
       <x:c r="F16" s="7" t="str">
         <x:f>IF(ABS(E16 - D16) &lt;= (D16 * 0.01), "Passed", "Failed")</x:f>
@@ -35191,7 +35191,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D24" s="7" t="n">
-        <x:v>1.2172493050419295</x:v>
+        <x:v>1.21724930504193</x:v>
       </x:c>
       <x:c r="F24" s="7" t="str">
         <x:f>IF(ABS(E24 - D24) &lt;= (D24 * 0.01), "Passed", "Failed")</x:f>
@@ -35329,7 +35329,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D8" s="7" t="n">
-        <x:v>110.93639217631153</x:v>
+        <x:v>110.936392176312</x:v>
       </x:c>
       <x:c r="F8" s="7" t="str">
         <x:f>IF(ABS(E8 - D8) &lt;= (D8 * 0.01), "Passed", "Failed")</x:f>
@@ -35375,7 +35375,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D12" s="7" t="n">
-        <x:v>110.93639217631153</x:v>
+        <x:v>110.936392176312</x:v>
       </x:c>
       <x:c r="F12" s="7" t="str">
         <x:f>IF(ABS(E12 - D12) &lt;= (D12 * 0.01), "Passed", "Failed")</x:f>
@@ -35510,7 +35510,7 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="D24" s="7" t="n">
-        <x:v>5.898445673784778</x:v>
+        <x:v>5.89844567378478</x:v>
       </x:c>
       <x:c r="F24" s="7" t="str">
         <x:f>IF(ABS(E24 - D24) &lt;= (D24 * 0.01), "Passed", "Failed")</x:f>

</xml_diff>